<commit_message>
adding HKD workbooks, getting rid of obosolate, migrating to Excel 2010
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
+++ b/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
@@ -15,9 +15,10 @@
     <sheet name="CHF" sheetId="6" r:id="rId6"/>
     <sheet name="HKD" sheetId="8" r:id="rId7"/>
     <sheet name="CAD" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="Currency" localSheetId="7">CAD!$E$3</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>Trigger</t>
   </si>
@@ -159,6 +160,21 @@
   </si>
   <si>
     <t>YCCCSBasis</t>
+  </si>
+  <si>
+    <t>HiborYC1M</t>
+  </si>
+  <si>
+    <t>HiborYC3M</t>
+  </si>
+  <si>
+    <t>HiborYC6M</t>
+  </si>
+  <si>
+    <t>HiborYC1Y</t>
+  </si>
+  <si>
+    <t>HiborYCON</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1068,7 @@
       </c>
       <c r="D8" s="21" t="str">
         <f>[1]!qlSerializationPath(Trigger)</f>
-        <v>X:\WorkGroup\IMI_Workbooks\Production\QLXL_R01030x\Data\XML\010_StartUp\010_RH\</v>
+        <v>\\srv0001\Risorse\WorkGroup\IMI_Workbooks\Production\QLXL_R01030x\Data\XML\010_StartUp\010_RH\</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="2"/>
@@ -2450,7 +2466,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurYC#0001</v>
+        <v>EurYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -2469,7 +2485,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurYCSTD#0001</v>
+        <v>EurYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -2488,7 +2504,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYCON#0001</v>
+        <v>EuriborYCON#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -2507,7 +2523,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1M#0001</v>
+        <v>EuriborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -2526,7 +2542,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC3M#0001</v>
+        <v>EuriborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -2545,7 +2561,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC6M#0001</v>
+        <v>EuriborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -2564,7 +2580,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1Y#0001</v>
+        <v>EuriborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -2584,7 +2600,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYCON-Mx#0001</v>
+        <v>EuriborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -2604,7 +2620,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1M-Mx#0001</v>
+        <v>EuriborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -2624,7 +2640,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC3M-Mx#0001</v>
+        <v>EuriborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -2644,7 +2660,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC6M-Mx#0001</v>
+        <v>EuriborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -2664,7 +2680,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1Y-Mx#0001</v>
+        <v>EuriborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -2683,7 +2699,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYCON#0001</v>
+        <v>EurLiborYCON#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -2702,7 +2718,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC1M#0001</v>
+        <v>EurLiborYC1M#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -2721,7 +2737,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC3M#0001</v>
+        <v>EurLiborYC3M#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -2740,7 +2756,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC6M#0001</v>
+        <v>EurLiborYC6M#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -2759,7 +2775,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC1Y#0001</v>
+        <v>EurLiborYC1Y#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -2803,7 +2819,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurSwaptionATMVol#0001</v>
+        <v>EurSwaptionATMVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -2822,7 +2838,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurSwaptionVol#0001</v>
+        <v>EurSwaptionVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -2866,7 +2882,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MFutOptionVol#0001</v>
+        <v>Eur3MFutOptionVol#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -2885,7 +2901,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1MCapletVol#0001</v>
+        <v>Eur1MCapletVol#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -2904,7 +2920,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MCapletVol#0001</v>
+        <v>Eur3MCapletVol#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -2923,7 +2939,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur6MCapletVol#0001</v>
+        <v>Eur6MCapletVol#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -2942,7 +2958,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1YCapletVol#0001</v>
+        <v>Eur1YCapletVol#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -2961,7 +2977,7 @@
       </c>
       <c r="E34" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D34,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MFutOptionVolEx#0001</v>
+        <v>Eur3MFutOptionVolEx#0002</v>
       </c>
       <c r="F34" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E34)</f>
@@ -2980,7 +2996,7 @@
       </c>
       <c r="E35" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D35,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1MCapletVolEx#0001</v>
+        <v>Eur1MCapletVolEx#0002</v>
       </c>
       <c r="F35" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E35)</f>
@@ -2999,7 +3015,7 @@
       </c>
       <c r="E36" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D36,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MCapletVolEx#0001</v>
+        <v>Eur3MCapletVolEx#0002</v>
       </c>
       <c r="F36" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E36)</f>
@@ -3018,7 +3034,7 @@
       </c>
       <c r="E37" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D37,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur6MCapletVolEx#0001</v>
+        <v>Eur6MCapletVolEx#0002</v>
       </c>
       <c r="F37" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E37)</f>
@@ -3037,7 +3053,7 @@
       </c>
       <c r="E38" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D38,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1YCapletVolEx#0001</v>
+        <v>Eur1YCapletVolEx#0002</v>
       </c>
       <c r="F38" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E38)</f>
@@ -3143,7 +3159,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdYC#0001</v>
+        <v>UsdYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -3162,7 +3178,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdYCSTD#0001</v>
+        <v>UsdYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -3181,7 +3197,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYCON#0001</v>
+        <v>UsdLiborYCON#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -3200,7 +3216,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1M#0001</v>
+        <v>UsdLiborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -3219,7 +3235,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC3M#0001</v>
+        <v>UsdLiborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -3238,7 +3254,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC6M#0001</v>
+        <v>UsdLiborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -3257,7 +3273,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1Y#0001</v>
+        <v>UsdLiborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -3277,7 +3293,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYCON-Mx#0001</v>
+        <v>UsdLiborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -3297,7 +3313,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1M-Mx#0001</v>
+        <v>UsdLiborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -3317,7 +3333,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC3M-Mx#0001</v>
+        <v>UsdLiborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -3337,7 +3353,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC6M-Mx#0001</v>
+        <v>UsdLiborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -3357,7 +3373,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1Y-Mx#0001</v>
+        <v>UsdLiborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -3401,7 +3417,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdSwaptionATMVol#0001</v>
+        <v>UsdSwaptionATMVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -3420,7 +3436,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdSwaptionVol#0001</v>
+        <v>UsdSwaptionVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -3464,7 +3480,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MFutOptionVol#0001</v>
+        <v>Usd3MFutOptionVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -3483,7 +3499,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1MCapletVol#0001</v>
+        <v>Usd1MCapletVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -3502,7 +3518,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MCapletVol#0001</v>
+        <v>Usd3MCapletVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -3521,7 +3537,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd6MCapletVol#0001</v>
+        <v>Usd6MCapletVol#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -3540,7 +3556,7 @@
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1YCapletVol#0001</v>
+        <v>Usd1YCapletVol#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -3559,7 +3575,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MFutOptionVolEx#0001</v>
+        <v>Usd3MFutOptionVolEx#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -3578,7 +3594,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1MCapletVolEx#0001</v>
+        <v>Usd1MCapletVolEx#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -3597,7 +3613,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MCapletVolEx#0001</v>
+        <v>Usd3MCapletVolEx#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -3616,7 +3632,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd6MCapletVolEx#0001</v>
+        <v>Usd6MCapletVolEx#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -3635,7 +3651,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1YCapletVolEx#0001</v>
+        <v>Usd1YCapletVolEx#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -3741,7 +3757,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpYC#0001</v>
+        <v>GbpYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -3760,7 +3776,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpYCSTD#0001</v>
+        <v>GbpYCSTD#0002</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="10"/>
@@ -3776,7 +3792,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYCON#0001</v>
+        <v>GbpLiborYCON#0002</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="10"/>
@@ -3792,7 +3808,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1M#0001</v>
+        <v>GbpLiborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -3811,7 +3827,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC3M#0001</v>
+        <v>GbpLiborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -3830,7 +3846,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC6M#0001</v>
+        <v>GbpLiborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -3849,7 +3865,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1Y#0001</v>
+        <v>GbpLiborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -3869,7 +3885,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYCON-Mx#0001</v>
+        <v>GbpLiborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -3889,7 +3905,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1M-Mx#0001</v>
+        <v>GbpLiborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -3909,7 +3925,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC3M-Mx#0001</v>
+        <v>GbpLiborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -3929,7 +3945,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC6M-Mx#0001</v>
+        <v>GbpLiborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -3949,7 +3965,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1Y-Mx#0001</v>
+        <v>GbpLiborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -3993,7 +4009,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpSwaptionATMVol#0001</v>
+        <v>GbpSwaptionATMVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -4012,7 +4028,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpSwaptionVol#0001</v>
+        <v>GbpSwaptionVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -4056,7 +4072,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MFutOptionVol#0001</v>
+        <v>Gbp3MFutOptionVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -4075,7 +4091,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1MCapletVol#0001</v>
+        <v>Gbp1MCapletVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -4094,7 +4110,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MCapletVol#0001</v>
+        <v>Gbp3MCapletVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -4113,7 +4129,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp6MCapletVol#0001</v>
+        <v>Gbp6MCapletVol#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -4132,7 +4148,7 @@
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1YCapletVol#0001</v>
+        <v>Gbp1YCapletVol#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -4151,7 +4167,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MFutOptionVolEx#0001</v>
+        <v>Gbp3MFutOptionVolEx#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -4170,7 +4186,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1MCapletVolEx#0001</v>
+        <v>Gbp1MCapletVolEx#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -4189,7 +4205,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MCapletVolEx#0001</v>
+        <v>Gbp3MCapletVolEx#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -4208,7 +4224,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp6MCapletVolEx#0001</v>
+        <v>Gbp6MCapletVolEx#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -4227,7 +4243,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1YCapletVolEx#0001</v>
+        <v>Gbp1YCapletVolEx#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -4333,7 +4349,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyYC#0001</v>
+        <v>JpyYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -4352,7 +4368,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC1M#0001</v>
+        <v>JpyLiborYC1M#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -4371,7 +4387,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC3M#0001</v>
+        <v>JpyLiborYC3M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -4390,7 +4406,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC6M#0001</v>
+        <v>JpyLiborYC6M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -4409,7 +4425,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC1Y#0001</v>
+        <v>JpyLiborYC1Y#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -4453,7 +4469,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpySwaptionATMVol#0001</v>
+        <v>JpySwaptionATMVol#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -4472,7 +4488,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpySwaptionVol#0001</v>
+        <v>JpySwaptionVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -4516,7 +4532,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MFutOptionVol#0001</v>
+        <v>Jpy3MFutOptionVol#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -4535,7 +4551,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1MCapletVol#0001</v>
+        <v>Jpy1MCapletVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -4554,7 +4570,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MCapletVol#0001</v>
+        <v>Jpy3MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -4573,7 +4589,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy6MCapletVol#0001</v>
+        <v>Jpy6MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -4592,7 +4608,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1YCapletVol#0001</v>
+        <v>Jpy1YCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -4611,7 +4627,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MFutOptionVolEx#0001</v>
+        <v>Jpy3MFutOptionVolEx#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -4630,7 +4646,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1MCapletVolEx#0001</v>
+        <v>Jpy1MCapletVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -4649,7 +4665,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MCapletVolEx#0001</v>
+        <v>Jpy3MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -4668,7 +4684,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy6MCapletVolEx#0001</v>
+        <v>Jpy6MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -4687,7 +4703,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1YCapletVolEx#0001</v>
+        <v>Jpy1YCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -4793,7 +4809,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfYC#0001</v>
+        <v>ChfYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -4812,7 +4828,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfYCSTD#0003</v>
+        <v>ChfYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -4831,7 +4847,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC1M#0001</v>
+        <v>ChfLiborYC1M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -4850,7 +4866,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC3M#0001</v>
+        <v>ChfLiborYC3M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -4869,7 +4885,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC6M#0001</v>
+        <v>ChfLiborYC6M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -4888,7 +4904,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC1Y#0001</v>
+        <v>ChfLiborYC1Y#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -4932,7 +4948,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfSwaptionATMVol#0001</v>
+        <v>ChfSwaptionATMVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -4951,7 +4967,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfSwaptionVol#0001</v>
+        <v>ChfSwaptionVol#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -4995,7 +5011,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MFutOptionVol#0001</v>
+        <v>Chf3MFutOptionVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -5014,7 +5030,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1MCapletVol#0001</v>
+        <v>Chf1MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -5033,7 +5049,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MCapletVol#0001</v>
+        <v>Chf3MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -5052,7 +5068,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf6MCapletVol#0001</v>
+        <v>Chf6MCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -5071,7 +5087,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1YCapletVol#0001</v>
+        <v>Chf1YCapletVol#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -5090,7 +5106,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MFutOptionVolEx#0001</v>
+        <v>Chf3MFutOptionVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -5109,7 +5125,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1MCapletVolEx#0001</v>
+        <v>Chf1MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -5128,7 +5144,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MCapletVolEx#0001</v>
+        <v>Chf3MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -5147,7 +5163,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf6MCapletVolEx#0001</v>
+        <v>Chf6MCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -5166,7 +5182,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1YCapletVolEx#0001</v>
+        <v>Chf1YCapletVolEx#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -5198,10 +5214,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="B1:G29"/>
+  <dimension ref="B1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5252,8 +5268,8 @@
         <v>HKD_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E12,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>7</v>
+        <f>IF(Serialize,_xll.ohObjectSave(E6:E13,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>8</v>
       </c>
       <c r="F5" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -5267,12 +5283,12 @@
         <v>8</v>
       </c>
       <c r="D6" s="17" t="str">
-        <f t="shared" ref="D6:D12" si="0">Currency&amp;C6</f>
+        <f t="shared" ref="D6:D13" si="0">Currency&amp;C6</f>
         <v>HkdYC</v>
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYC#0003</v>
+        <v>HkdYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -5291,7 +5307,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYCSTD#0003</v>
+        <v>HkdYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -5310,7 +5326,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYCCCSBasis#0001</v>
+        <v>HkdYCCCSBasis#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -5321,15 +5337,15 @@
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="17" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D9" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>HkdLiborYC1M</v>
+        <f t="shared" ref="D9" si="1">Currency&amp;C9</f>
+        <v>HkdHiborYCON</v>
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdLiborYC1M#0003</v>
+        <v>HkdHiborYCON#0003</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -5340,15 +5356,15 @@
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="17" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D10" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>HkdLiborYC3M</v>
+        <v>HkdHiborYC1M</v>
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdLiborYC3M#0003</v>
+        <v>HkdHiborYC1M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -5359,15 +5375,15 @@
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="17" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D11" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>HkdLiborYC6M</v>
+        <v>HkdHiborYC3M</v>
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdLiborYC6M#0003</v>
+        <v>HkdHiborYC3M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -5378,15 +5394,15 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="17" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D12" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>HkdLiborYC1Y</v>
+        <v>HkdHiborYC6M</v>
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdLiborYC1Y#0003</v>
+        <v>HkdHiborYC6M#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -5396,41 +5412,41 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="C13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>HkdHiborYC1Y</v>
+      </c>
+      <c r="E13" s="18" t="str">
+        <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HkdHiborYC1Y#0002</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <f>_xll.ohRangeRetrieveError(E13)</f>
+        <v/>
+      </c>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
       <c r="C14" s="24"/>
-      <c r="D14" s="23" t="str">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="8"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="23" t="str">
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>HKD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E14" s="22">
-        <f>IF(Serialize,_xll.ohObjectSave(E15:E16,SerializationPath&amp;D14,FileOverwrite,Serialize),"---")</f>
+      <c r="E15" s="22">
+        <f>IF(Serialize,_xll.ohObjectSave(E16:E17,SerializationPath&amp;D15,FileOverwrite,Serialize),"---")</f>
         <v>2</v>
-      </c>
-      <c r="F14" s="20" t="str">
-        <f>_xll.ohRangeRetrieveError(E14)</f>
-        <v/>
-      </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="8"/>
-      <c r="C15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="17" t="str">
-        <f>Currency&amp;C15</f>
-        <v>HkdSwaptionATMVol</v>
-      </c>
-      <c r="E15" s="18" t="str">
-        <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdSwaptionATMVol#0003</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -5441,15 +5457,15 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" s="17" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D16" s="17" t="str">
         <f>Currency&amp;C16</f>
-        <v>HkdSwaptionVol</v>
+        <v>HkdSwaptionATMVol</v>
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdSwaptionVol#0003</v>
+        <v>HkdSwaptionATMVol#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -5459,41 +5475,41 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="C17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17" t="str">
+        <f>Currency&amp;C17</f>
+        <v>HkdSwaptionVol</v>
+      </c>
+      <c r="E17" s="18" t="str">
+        <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HkdSwaptionVol#0002</v>
+      </c>
+      <c r="F17" s="20" t="str">
+        <f>_xll.ohRangeRetrieveError(E17)</f>
+        <v/>
+      </c>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="23" t="str">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23" t="str">
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>HKD_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E18" s="22">
-        <f>IF(Serialize,_xll.ohObjectSave(E19:E28,SerializationPath&amp;D18,FileOverwrite,Serialize),"---")</f>
+      <c r="E19" s="22">
+        <f>IF(Serialize,_xll.ohObjectSave(E20:E29,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
         <v>10</v>
-      </c>
-      <c r="F18" s="20" t="str">
-        <f>_xll.ohRangeRetrieveError(E18)</f>
-        <v/>
-      </c>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="17" t="str">
-        <f t="shared" ref="D19:D28" si="1">Currency&amp;C19</f>
-        <v>Hkd3MFutOptionVol</v>
-      </c>
-      <c r="E19" s="18" t="str">
-        <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MFutOptionVol#0003</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -5504,15 +5520,15 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd1MCapletVol</v>
+        <f t="shared" ref="D20:D29" si="2">Currency&amp;C20</f>
+        <v>Hkd3MFutOptionVol</v>
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1MCapletVol#0003</v>
+        <v>Hkd3MFutOptionVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -5523,15 +5539,15 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd3MCapletVol</v>
+        <f t="shared" si="2"/>
+        <v>Hkd1MCapletVol</v>
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MCapletVol#0003</v>
+        <v>Hkd1MCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -5542,15 +5558,15 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd6MCapletVol</v>
+        <f t="shared" si="2"/>
+        <v>Hkd3MCapletVol</v>
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd6MCapletVol#0003</v>
+        <v>Hkd3MCapletVol#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -5561,15 +5577,15 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
       <c r="C23" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd1YCapletVol</v>
+        <f t="shared" si="2"/>
+        <v>Hkd6MCapletVol</v>
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1YCapletVol#0003</v>
+        <v>Hkd6MCapletVol#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -5580,15 +5596,15 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
       <c r="C24" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd3MFutOptionVolEx</v>
+        <f t="shared" si="2"/>
+        <v>Hkd1YCapletVol</v>
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MFutOptionVolEx#0003</v>
+        <v>Hkd1YCapletVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -5599,15 +5615,15 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
       <c r="C25" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd1MCapletVolEx</v>
+        <f t="shared" si="2"/>
+        <v>Hkd3MFutOptionVolEx</v>
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1MCapletVolEx#0003</v>
+        <v>Hkd3MFutOptionVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -5618,15 +5634,15 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd3MCapletVolEx</v>
+        <f t="shared" si="2"/>
+        <v>Hkd1MCapletVolEx</v>
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MCapletVolEx#0003</v>
+        <v>Hkd1MCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -5637,15 +5653,15 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd6MCapletVolEx</v>
+        <f t="shared" si="2"/>
+        <v>Hkd3MCapletVolEx</v>
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd6MCapletVolEx#0003</v>
+        <v>Hkd3MCapletVolEx#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -5656,15 +5672,15 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="C28" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Hkd1YCapletVolEx</v>
+        <f t="shared" si="2"/>
+        <v>Hkd6MCapletVolEx</v>
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1YCapletVolEx#0003</v>
+        <v>Hkd6MCapletVolEx#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -5672,13 +5688,32 @@
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="13"/>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="8"/>
+      <c r="C29" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Hkd1YCapletVolEx</v>
+      </c>
+      <c r="E29" s="18" t="str">
+        <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>Hkd1YCapletVolEx#0002</v>
+      </c>
+      <c r="F29" s="20" t="str">
+        <f>_xll.ohRangeRetrieveError(E29)</f>
+        <v/>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5770,7 +5805,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadYC#0001</v>
+        <v>CadYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -5789,7 +5824,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC1M#0001</v>
+        <v>CadLiborYC1M#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -5808,7 +5843,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC3M#0001</v>
+        <v>CadLiborYC3M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -5827,7 +5862,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC6M#0001</v>
+        <v>CadLiborYC6M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -5846,7 +5881,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC1Y#0001</v>
+        <v>CadLiborYC1Y#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -5890,7 +5925,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadSwaptionATMVol#0001</v>
+        <v>CadSwaptionATMVol#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -5909,7 +5944,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadSwaptionVol#0001</v>
+        <v>CadSwaptionVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -5953,7 +5988,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MFutOptionVol#0001</v>
+        <v>Cad3MFutOptionVol#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -5972,7 +6007,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1MCapletVol#0001</v>
+        <v>Cad1MCapletVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -5991,7 +6026,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MCapletVol#0001</v>
+        <v>Cad3MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -6010,7 +6045,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad6MCapletVol#0001</v>
+        <v>Cad6MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -6029,7 +6064,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1YCapletVol#0001</v>
+        <v>Cad1YCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -6048,7 +6083,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MFutOptionVolEx#0001</v>
+        <v>Cad3MFutOptionVolEx#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -6067,7 +6102,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1MCapletVolEx#0001</v>
+        <v>Cad1MCapletVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -6086,7 +6121,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MCapletVolEx#0001</v>
+        <v>Cad3MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -6105,7 +6140,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad6MCapletVolEx#0001</v>
+        <v>Cad6MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -6124,7 +6159,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1YCapletVolEx#0001</v>
+        <v>Cad1YCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -6151,4 +6186,17 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove links from workbooks to FixedIncome.xla
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
+++ b/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
@@ -17,9 +17,6 @@
     <sheet name="CAD" sheetId="9" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Currency" localSheetId="7">CAD!$E$3</definedName>
     <definedName name="Currency" localSheetId="5">CHF!$E$3</definedName>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
   <si>
     <t>Trigger</t>
   </si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>HiborYCON</t>
+  </si>
+  <si>
+    <t>C:\Users\erik\junk\</t>
   </si>
 </sst>
 </file>
@@ -503,22 +503,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="qlSerializationPath"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1066,9 +1050,8 @@
       <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="21" t="str">
-        <f>[1]!qlSerializationPath(Trigger)</f>
-        <v>C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\</v>
+      <c r="D8" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="2"/>
@@ -2451,7 +2434,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\EUR_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -2804,7 +2787,7 @@
       </c>
       <c r="F24" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E24)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\EUR_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -2867,7 +2850,7 @@
       </c>
       <c r="F28" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E28)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\EUR_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -3144,7 +3127,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\USD_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3402,7 +3385,7 @@
       </c>
       <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\USD_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -3465,7 +3448,7 @@
       </c>
       <c r="F23" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\USD_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -3742,7 +3725,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\GBP_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3994,7 +3977,7 @@
       </c>
       <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\GBP_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -4057,7 +4040,7 @@
       </c>
       <c r="F23" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\GBP_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -4334,7 +4317,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\JPY_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4454,7 +4437,7 @@
       </c>
       <c r="F12" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\JPY_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -4517,7 +4500,7 @@
       </c>
       <c r="F16" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\JPY_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -4794,7 +4777,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CHF_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4933,7 +4916,7 @@
       </c>
       <c r="F13" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E13)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CHF_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -4996,7 +4979,7 @@
       </c>
       <c r="F17" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E17)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CHF_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -5273,7 +5256,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\HKD_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5450,7 +5433,7 @@
       </c>
       <c r="F15" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E15)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\HKD_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -5513,7 +5496,7 @@
       </c>
       <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\HKD_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -5790,7 +5773,7 @@
       </c>
       <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CAD_RH_YieldTermStructure.xml</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5910,7 +5893,7 @@
       </c>
       <c r="F12" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CAD_RH_SwaptionVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -5973,7 +5956,7 @@
       </c>
       <c r="F16" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v>ohObjectSave - Invalid parent path : C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\CAD_RH_OptionletVolatilityStructure.xml</v>
+        <v/>
       </c>
       <c r="G16" s="10"/>
     </row>

</xml_diff>

<commit_message>
update workbooks to calculate their own serialization paths
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
+++ b/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>Trigger</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>HiborYCON</t>
-  </si>
-  <si>
-    <t>C:\Users\erik\junk\</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1047,9 @@
       <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>45</v>
+      <c r="D8" s="21" t="str">
+        <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
+        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data\XML\010_StartUp\010_RH\</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="2"/>
@@ -2429,12 +2427,12 @@
         <v>EUR_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E22,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E22,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -2782,12 +2780,12 @@
         <v>EUR_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E24" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E25:E26,SerializationPath&amp;D24,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F24" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E25:E26,SerializationPath&amp;D24,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F24" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E24)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -2845,12 +2843,12 @@
         <v>EUR_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E28" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E29:E38,SerializationPath&amp;D28,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F28" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E29:E38,SerializationPath&amp;D28,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F28" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E28)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -3122,12 +3120,12 @@
         <v>USD_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3380,12 +3378,12 @@
         <v>USD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E19" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F19" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F19" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -3443,12 +3441,12 @@
         <v>USD_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E23" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F23" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F23" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -3720,12 +3718,12 @@
         <v>GBP_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3972,12 +3970,12 @@
         <v>GBP_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E19" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F19" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F19" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -4035,12 +4033,12 @@
         <v>GBP_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E23" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F23" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F23" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -4312,12 +4310,12 @@
         <v>JPY_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4432,12 +4430,12 @@
         <v>JPY_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E12" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F12" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -4495,12 +4493,12 @@
         <v>JPY_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E16" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F16" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F16" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -4772,12 +4770,12 @@
         <v>CHF_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E11,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E11,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4911,12 +4909,12 @@
         <v>CHF_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E13" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E14:E15,SerializationPath&amp;D13,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F13" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E14:E15,SerializationPath&amp;D13,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F13" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E13)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -4974,12 +4972,12 @@
         <v>CHF_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E17" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E18:E27,SerializationPath&amp;D17,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F17" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E18:E27,SerializationPath&amp;D17,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F17" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E17)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -5251,12 +5249,12 @@
         <v>HKD_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E13,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E13,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5428,12 +5426,12 @@
         <v>HKD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E15" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E16:E17,SerializationPath&amp;D15,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F15" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E16:E17,SerializationPath&amp;D15,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F15" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E15)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -5491,12 +5489,12 @@
         <v>HKD_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E19" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E20:E29,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F19" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E29,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F19" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -5768,12 +5766,12 @@
         <v>CAD_RH_YieldTermStructure.xml</v>
       </c>
       <c r="E5" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5888,12 +5886,12 @@
         <v>CAD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
       <c r="E12" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F12" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -5951,12 +5949,12 @@
         <v>CAD_RH_OptionletVolatilityStructure.xml</v>
       </c>
       <c r="E16" s="22" t="e">
-        <f>IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F16" s="20" t="str">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F16" s="20" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="G16" s="10"/>
     </row>

</xml_diff>

<commit_message>
dynamic xlls + proper serialize() parameter order
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
+++ b/QuantLibXL/Data/XLS/010_StartUp/010_RH/RelinkableHandles.xlsx
@@ -15,7 +15,6 @@
     <sheet name="CHF" sheetId="6" r:id="rId6"/>
     <sheet name="HKD" sheetId="8" r:id="rId7"/>
     <sheet name="CAD" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Currency" localSheetId="7">CAD!$E$3</definedName>
@@ -809,7 +808,7 @@
       <c r="A1" s="14"/>
       <c r="B1" s="14" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov  4 2013 11:55:45</v>
+        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Nov  6 2013 01:01:46</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1049,7 +1048,7 @@
       </c>
       <c r="D8" s="21" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data\XML\010_StartUp\010_RH\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data\XML\010_StartUp\010_RH\</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="2"/>
@@ -2426,13 +2425,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>EUR_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E22,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E22,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>17</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -2447,7 +2446,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurYC#0001</v>
+        <v>EurYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -2466,7 +2465,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurYCSTD#0001</v>
+        <v>EurYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -2485,7 +2484,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYCON#0001</v>
+        <v>EuriborYCON#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -2504,7 +2503,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1M#0001</v>
+        <v>EuriborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -2523,7 +2522,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC3M#0001</v>
+        <v>EuriborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -2542,7 +2541,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC6M#0001</v>
+        <v>EuriborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -2561,7 +2560,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1Y#0001</v>
+        <v>EuriborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -2581,7 +2580,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYCON-Mx#0001</v>
+        <v>EuriborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -2601,7 +2600,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1M-Mx#0001</v>
+        <v>EuriborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -2621,7 +2620,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC3M-Mx#0001</v>
+        <v>EuriborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -2641,7 +2640,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC6M-Mx#0001</v>
+        <v>EuriborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -2661,7 +2660,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EuriborYC1Y-Mx#0001</v>
+        <v>EuriborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -2680,7 +2679,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYCON#0001</v>
+        <v>EurLiborYCON#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -2699,7 +2698,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC1M#0001</v>
+        <v>EurLiborYC1M#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -2718,7 +2717,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC3M#0001</v>
+        <v>EurLiborYC3M#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -2737,7 +2736,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC6M#0001</v>
+        <v>EurLiborYC6M#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -2756,7 +2755,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurLiborYC1Y#0001</v>
+        <v>EurLiborYC1Y#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -2779,13 +2778,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>EUR_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E24" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E25:E26,SerializationPath&amp;D24,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F24" s="20" t="e">
+      <c r="E24" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E25:E26,SerializationPath&amp;D24,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E24)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -2800,7 +2799,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurSwaptionATMVol#0001</v>
+        <v>EurSwaptionATMVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -2819,7 +2818,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EurSwaptionVol#0001</v>
+        <v>EurSwaptionVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -2842,13 +2841,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>EUR_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E28" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E29:E38,SerializationPath&amp;D28,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F28" s="20" t="e">
+      <c r="E28" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E29:E38,SerializationPath&amp;D28,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F28" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E28)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -2863,7 +2862,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MFutOptionVol#0001</v>
+        <v>Eur3MFutOptionVol#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -2882,7 +2881,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1MCapletVol#0001</v>
+        <v>Eur1MCapletVol#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -2901,7 +2900,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MCapletVol#0001</v>
+        <v>Eur3MCapletVol#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -2920,7 +2919,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur6MCapletVol#0001</v>
+        <v>Eur6MCapletVol#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -2939,7 +2938,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1YCapletVol#0001</v>
+        <v>Eur1YCapletVol#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -2958,7 +2957,7 @@
       </c>
       <c r="E34" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D34,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MFutOptionVolEx#0001</v>
+        <v>Eur3MFutOptionVolEx#0002</v>
       </c>
       <c r="F34" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E34)</f>
@@ -2977,7 +2976,7 @@
       </c>
       <c r="E35" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D35,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1MCapletVolEx#0001</v>
+        <v>Eur1MCapletVolEx#0002</v>
       </c>
       <c r="F35" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E35)</f>
@@ -2996,7 +2995,7 @@
       </c>
       <c r="E36" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D36,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur3MCapletVolEx#0001</v>
+        <v>Eur3MCapletVolEx#0002</v>
       </c>
       <c r="F36" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E36)</f>
@@ -3015,7 +3014,7 @@
       </c>
       <c r="E37" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D37,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur6MCapletVolEx#0001</v>
+        <v>Eur6MCapletVolEx#0002</v>
       </c>
       <c r="F37" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E37)</f>
@@ -3034,7 +3033,7 @@
       </c>
       <c r="E38" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D38,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Eur1YCapletVolEx#0001</v>
+        <v>Eur1YCapletVolEx#0002</v>
       </c>
       <c r="F38" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E38)</f>
@@ -3069,7 +3068,7 @@
   <dimension ref="B1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3119,13 +3118,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>USD_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3140,7 +3139,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdYC#0001</v>
+        <v>UsdYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -3159,7 +3158,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdYCSTD#0001</v>
+        <v>UsdYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -3178,7 +3177,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYCON#0001</v>
+        <v>UsdLiborYCON#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -3197,7 +3196,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1M#0001</v>
+        <v>UsdLiborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -3216,7 +3215,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC3M#0001</v>
+        <v>UsdLiborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -3235,7 +3234,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC6M#0001</v>
+        <v>UsdLiborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -3254,7 +3253,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1Y#0001</v>
+        <v>UsdLiborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -3274,7 +3273,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYCON-Mx#0001</v>
+        <v>UsdLiborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -3294,7 +3293,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1M-Mx#0001</v>
+        <v>UsdLiborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -3314,7 +3313,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC3M-Mx#0001</v>
+        <v>UsdLiborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -3334,7 +3333,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC6M-Mx#0001</v>
+        <v>UsdLiborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -3354,7 +3353,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdLiborYC1Y-Mx#0001</v>
+        <v>UsdLiborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -3377,13 +3376,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>USD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E19" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F19" s="20" t="e">
+      <c r="E19" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -3398,7 +3397,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdSwaptionATMVol#0001</v>
+        <v>UsdSwaptionATMVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -3417,7 +3416,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>UsdSwaptionVol#0001</v>
+        <v>UsdSwaptionVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -3440,13 +3439,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>USD_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E23" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F23" s="20" t="e">
+      <c r="E23" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F23" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -3461,7 +3460,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MFutOptionVol#0001</v>
+        <v>Usd3MFutOptionVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -3480,7 +3479,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1MCapletVol#0001</v>
+        <v>Usd1MCapletVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -3499,7 +3498,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MCapletVol#0001</v>
+        <v>Usd3MCapletVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -3518,7 +3517,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd6MCapletVol#0001</v>
+        <v>Usd6MCapletVol#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -3537,7 +3536,7 @@
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1YCapletVol#0001</v>
+        <v>Usd1YCapletVol#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -3556,7 +3555,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MFutOptionVolEx#0001</v>
+        <v>Usd3MFutOptionVolEx#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -3575,7 +3574,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1MCapletVolEx#0001</v>
+        <v>Usd1MCapletVolEx#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -3594,7 +3593,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd3MCapletVolEx#0001</v>
+        <v>Usd3MCapletVolEx#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -3613,7 +3612,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd6MCapletVolEx#0001</v>
+        <v>Usd6MCapletVolEx#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -3632,7 +3631,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Usd1YCapletVolEx#0001</v>
+        <v>Usd1YCapletVolEx#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -3717,13 +3716,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>GBP_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E17,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -3738,7 +3737,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpYC#0001</v>
+        <v>GbpYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -3757,7 +3756,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpYCSTD#0001</v>
+        <v>GbpYCSTD#0002</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="10"/>
@@ -3773,7 +3772,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYCON#0001</v>
+        <v>GbpLiborYCON#0002</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="10"/>
@@ -3789,7 +3788,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1M#0001</v>
+        <v>GbpLiborYC1M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -3808,7 +3807,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC3M#0001</v>
+        <v>GbpLiborYC3M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -3827,7 +3826,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC6M#0001</v>
+        <v>GbpLiborYC6M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -3846,7 +3845,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1Y#0001</v>
+        <v>GbpLiborYC1Y#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -3866,7 +3865,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYCON-Mx#0001</v>
+        <v>GbpLiborYCON-Mx#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -3886,7 +3885,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1M-Mx#0001</v>
+        <v>GbpLiborYC1M-Mx#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -3906,7 +3905,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC3M-Mx#0001</v>
+        <v>GbpLiborYC3M-Mx#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -3926,7 +3925,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC6M-Mx#0001</v>
+        <v>GbpLiborYC6M-Mx#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -3946,7 +3945,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpLiborYC1Y-Mx#0001</v>
+        <v>GbpLiborYC1Y-Mx#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -3969,13 +3968,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>GBP_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E19" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F19" s="20" t="e">
+      <c r="E19" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E21,SerializationPath&amp;D19,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -3990,7 +3989,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpSwaptionATMVol#0001</v>
+        <v>GbpSwaptionATMVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -4009,7 +4008,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GbpSwaptionVol#0001</v>
+        <v>GbpSwaptionVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -4032,13 +4031,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>GBP_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E23" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F23" s="20" t="e">
+      <c r="E23" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E24:E33,SerializationPath&amp;D23,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F23" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E23)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -4053,7 +4052,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MFutOptionVol#0001</v>
+        <v>Gbp3MFutOptionVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -4072,7 +4071,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1MCapletVol#0001</v>
+        <v>Gbp1MCapletVol#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -4091,7 +4090,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MCapletVol#0001</v>
+        <v>Gbp3MCapletVol#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -4110,7 +4109,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp6MCapletVol#0001</v>
+        <v>Gbp6MCapletVol#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -4129,7 +4128,7 @@
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1YCapletVol#0001</v>
+        <v>Gbp1YCapletVol#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -4148,7 +4147,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MFutOptionVolEx#0001</v>
+        <v>Gbp3MFutOptionVolEx#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -4167,7 +4166,7 @@
       </c>
       <c r="E30" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D30,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1MCapletVolEx#0001</v>
+        <v>Gbp1MCapletVolEx#0002</v>
       </c>
       <c r="F30" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E30)</f>
@@ -4186,7 +4185,7 @@
       </c>
       <c r="E31" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D31,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp3MCapletVolEx#0001</v>
+        <v>Gbp3MCapletVolEx#0002</v>
       </c>
       <c r="F31" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E31)</f>
@@ -4205,7 +4204,7 @@
       </c>
       <c r="E32" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D32,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp6MCapletVolEx#0001</v>
+        <v>Gbp6MCapletVolEx#0002</v>
       </c>
       <c r="F32" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E32)</f>
@@ -4224,7 +4223,7 @@
       </c>
       <c r="E33" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D33,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Gbp1YCapletVolEx#0001</v>
+        <v>Gbp1YCapletVolEx#0002</v>
       </c>
       <c r="F33" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E33)</f>
@@ -4309,13 +4308,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>JPY_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4330,7 +4329,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyYC#0001</v>
+        <v>JpyYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -4349,7 +4348,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC1M#0001</v>
+        <v>JpyLiborYC1M#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -4368,7 +4367,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC3M#0001</v>
+        <v>JpyLiborYC3M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -4387,7 +4386,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC6M#0001</v>
+        <v>JpyLiborYC6M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -4406,7 +4405,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpyLiborYC1Y#0001</v>
+        <v>JpyLiborYC1Y#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -4429,13 +4428,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>JPY_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E12" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F12" s="20" t="e">
+      <c r="E12" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -4450,7 +4449,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpySwaptionATMVol#0001</v>
+        <v>JpySwaptionATMVol#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -4469,7 +4468,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>JpySwaptionVol#0001</v>
+        <v>JpySwaptionVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -4492,13 +4491,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>JPY_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E16" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F16" s="20" t="e">
+      <c r="E16" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -4513,7 +4512,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MFutOptionVol#0001</v>
+        <v>Jpy3MFutOptionVol#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -4532,7 +4531,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1MCapletVol#0001</v>
+        <v>Jpy1MCapletVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -4551,7 +4550,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MCapletVol#0001</v>
+        <v>Jpy3MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -4570,7 +4569,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy6MCapletVol#0001</v>
+        <v>Jpy6MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -4589,7 +4588,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1YCapletVol#0001</v>
+        <v>Jpy1YCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -4608,7 +4607,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MFutOptionVolEx#0001</v>
+        <v>Jpy3MFutOptionVolEx#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -4627,7 +4626,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1MCapletVolEx#0001</v>
+        <v>Jpy1MCapletVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -4646,7 +4645,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy3MCapletVolEx#0001</v>
+        <v>Jpy3MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -4665,7 +4664,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy6MCapletVolEx#0001</v>
+        <v>Jpy6MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -4684,7 +4683,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Jpy1YCapletVolEx#0001</v>
+        <v>Jpy1YCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -4769,13 +4768,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>CHF_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E11,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E11,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>6</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -4790,7 +4789,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfYC#0001</v>
+        <v>ChfYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -4809,7 +4808,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfYCSTD#0001</v>
+        <v>ChfYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -4828,7 +4827,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC1M#0001</v>
+        <v>ChfLiborYC1M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -4847,7 +4846,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC3M#0001</v>
+        <v>ChfLiborYC3M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -4866,7 +4865,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC6M#0001</v>
+        <v>ChfLiborYC6M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -4885,7 +4884,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfLiborYC1Y#0001</v>
+        <v>ChfLiborYC1Y#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -4908,13 +4907,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>CHF_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E13" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E14:E15,SerializationPath&amp;D13,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F13" s="20" t="e">
+      <c r="E13" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E14:E15,SerializationPath&amp;D13,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F13" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E13)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -4929,7 +4928,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfSwaptionATMVol#0001</v>
+        <v>ChfSwaptionATMVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -4948,7 +4947,7 @@
       </c>
       <c r="E15" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D15,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>ChfSwaptionVol#0001</v>
+        <v>ChfSwaptionVol#0002</v>
       </c>
       <c r="F15" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -4971,13 +4970,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>CHF_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E17" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E18:E27,SerializationPath&amp;D17,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F17" s="20" t="e">
+      <c r="E17" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E18:E27,SerializationPath&amp;D17,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E17)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -4992,7 +4991,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MFutOptionVol#0001</v>
+        <v>Chf3MFutOptionVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -5011,7 +5010,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1MCapletVol#0001</v>
+        <v>Chf1MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -5030,7 +5029,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MCapletVol#0001</v>
+        <v>Chf3MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -5049,7 +5048,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf6MCapletVol#0001</v>
+        <v>Chf6MCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -5068,7 +5067,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1YCapletVol#0001</v>
+        <v>Chf1YCapletVol#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -5087,7 +5086,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MFutOptionVolEx#0001</v>
+        <v>Chf3MFutOptionVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -5106,7 +5105,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1MCapletVolEx#0001</v>
+        <v>Chf1MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -5125,7 +5124,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf3MCapletVolEx#0001</v>
+        <v>Chf3MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -5144,7 +5143,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf6MCapletVolEx#0001</v>
+        <v>Chf6MCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -5163,7 +5162,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Chf1YCapletVolEx#0001</v>
+        <v>Chf1YCapletVolEx#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -5248,13 +5247,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>HKD_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E13,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E13,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5269,7 +5268,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYC#0001</v>
+        <v>HkdYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -5288,7 +5287,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYCSTD#0001</v>
+        <v>HkdYCSTD#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -5307,7 +5306,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdYCCCSBasis#0001</v>
+        <v>HkdYCCCSBasis#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -5326,7 +5325,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborYCON#0001</v>
+        <v>HkdHiborYCON#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -5345,7 +5344,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborYC1M#0001</v>
+        <v>HkdHiborYC1M#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -5364,7 +5363,7 @@
       </c>
       <c r="E11" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborYC3M#0001</v>
+        <v>HkdHiborYC3M#0002</v>
       </c>
       <c r="F11" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -5383,7 +5382,7 @@
       </c>
       <c r="E12" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D12,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborYC6M#0001</v>
+        <v>HkdHiborYC6M#0002</v>
       </c>
       <c r="F12" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -5402,7 +5401,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborYC1Y#0001</v>
+        <v>HkdHiborYC1Y#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -5425,13 +5424,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>HKD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E15" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E16:E17,SerializationPath&amp;D15,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F15" s="20" t="e">
+      <c r="E15" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E16:E17,SerializationPath&amp;D15,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E15)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -5446,7 +5445,7 @@
       </c>
       <c r="E16" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D16,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdSwaptionATMVol#0001</v>
+        <v>HkdSwaptionATMVol#0002</v>
       </c>
       <c r="F16" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -5465,7 +5464,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdSwaptionVol#0001</v>
+        <v>HkdSwaptionVol#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -5488,13 +5487,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>HKD_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E19" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E29,SerializationPath&amp;D19,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F19" s="20" t="e">
+      <c r="E19" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E20:E29,SerializationPath&amp;D19,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F19" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E19)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -5509,7 +5508,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MFutOptionVol#0001</v>
+        <v>Hkd3MFutOptionVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -5528,7 +5527,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1MCapletVol#0001</v>
+        <v>Hkd1MCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -5547,7 +5546,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MCapletVol#0001</v>
+        <v>Hkd3MCapletVol#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -5566,7 +5565,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd6MCapletVol#0001</v>
+        <v>Hkd6MCapletVol#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -5585,7 +5584,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1YCapletVol#0001</v>
+        <v>Hkd1YCapletVol#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -5604,7 +5603,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MFutOptionVolEx#0001</v>
+        <v>Hkd3MFutOptionVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -5623,7 +5622,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1MCapletVolEx#0001</v>
+        <v>Hkd1MCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -5642,7 +5641,7 @@
       </c>
       <c r="E27" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D27,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd3MCapletVolEx#0001</v>
+        <v>Hkd3MCapletVolEx#0002</v>
       </c>
       <c r="F27" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E27)</f>
@@ -5661,7 +5660,7 @@
       </c>
       <c r="E28" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D28,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd6MCapletVolEx#0001</v>
+        <v>Hkd6MCapletVolEx#0002</v>
       </c>
       <c r="F28" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E28)</f>
@@ -5680,7 +5679,7 @@
       </c>
       <c r="E29" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D29,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Hkd1YCapletVolEx#0001</v>
+        <v>Hkd1YCapletVolEx#0002</v>
       </c>
       <c r="F29" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E29)</f>
@@ -5765,13 +5764,13 @@
         <f>UPPER(Currency)&amp;"_RH_YieldTermStructure.xml"</f>
         <v>CAD_RH_YieldTermStructure.xml</v>
       </c>
-      <c r="E5" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="20" t="e">
+      <c r="E5" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E6:E10,SerializationPath&amp;D5,FileOverwrite,,Serialize),"---")</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E5)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -5786,7 +5785,7 @@
       </c>
       <c r="E6" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadYC#0001</v>
+        <v>CadYC#0002</v>
       </c>
       <c r="F6" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -5805,7 +5804,7 @@
       </c>
       <c r="E7" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC1M#0001</v>
+        <v>CadLiborYC1M#0002</v>
       </c>
       <c r="F7" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -5824,7 +5823,7 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC3M#0001</v>
+        <v>CadLiborYC3M#0002</v>
       </c>
       <c r="F8" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -5843,7 +5842,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC6M#0001</v>
+        <v>CadLiborYC6M#0002</v>
       </c>
       <c r="F9" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -5862,7 +5861,7 @@
       </c>
       <c r="E10" s="18" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(D10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadLiborYC1Y#0001</v>
+        <v>CadLiborYC1Y#0002</v>
       </c>
       <c r="F10" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -5885,13 +5884,13 @@
         <f>UPPER(Currency)&amp;"_RH_SwaptionVolatilityStructure.xml"</f>
         <v>CAD_RH_SwaptionVolatilityStructure.xml</v>
       </c>
-      <c r="E12" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F12" s="20" t="e">
+      <c r="E12" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E13:E14,SerializationPath&amp;D12,FileOverwrite,,Serialize),"---")</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E12)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -5906,7 +5905,7 @@
       </c>
       <c r="E13" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D13,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadSwaptionATMVol#0001</v>
+        <v>CadSwaptionATMVol#0002</v>
       </c>
       <c r="F13" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -5925,7 +5924,7 @@
       </c>
       <c r="E14" s="18" t="str">
         <f>_xll.qlRelinkableHandleSwaptionVolatilityStructure(D14,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>CadSwaptionVol#0001</v>
+        <v>CadSwaptionVol#0002</v>
       </c>
       <c r="F14" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -5948,13 +5947,13 @@
         <f>UPPER(Currency)&amp;"_RH_OptionletVolatilityStructure.xml"</f>
         <v>CAD_RH_OptionletVolatilityStructure.xml</v>
       </c>
-      <c r="E16" s="22" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,Serialize),"---")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F16" s="20" t="e">
+      <c r="E16" s="22">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(E17:E26,SerializationPath&amp;D16,FileOverwrite,,Serialize),"---")</f>
+        <v>10</v>
+      </c>
+      <c r="F16" s="20" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(E16)</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -5969,7 +5968,7 @@
       </c>
       <c r="E17" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D17,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MFutOptionVol#0001</v>
+        <v>Cad3MFutOptionVol#0002</v>
       </c>
       <c r="F17" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -5988,7 +5987,7 @@
       </c>
       <c r="E18" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D18,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1MCapletVol#0001</v>
+        <v>Cad1MCapletVol#0002</v>
       </c>
       <c r="F18" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -6007,7 +6006,7 @@
       </c>
       <c r="E19" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D19,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MCapletVol#0001</v>
+        <v>Cad3MCapletVol#0002</v>
       </c>
       <c r="F19" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -6026,7 +6025,7 @@
       </c>
       <c r="E20" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D20,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad6MCapletVol#0001</v>
+        <v>Cad6MCapletVol#0002</v>
       </c>
       <c r="F20" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -6045,7 +6044,7 @@
       </c>
       <c r="E21" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D21,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1YCapletVol#0001</v>
+        <v>Cad1YCapletVol#0002</v>
       </c>
       <c r="F21" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -6064,7 +6063,7 @@
       </c>
       <c r="E22" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D22,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MFutOptionVolEx#0001</v>
+        <v>Cad3MFutOptionVolEx#0002</v>
       </c>
       <c r="F22" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -6083,7 +6082,7 @@
       </c>
       <c r="E23" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D23,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1MCapletVolEx#0001</v>
+        <v>Cad1MCapletVolEx#0002</v>
       </c>
       <c r="F23" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -6102,7 +6101,7 @@
       </c>
       <c r="E24" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D24,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad3MCapletVolEx#0001</v>
+        <v>Cad3MCapletVolEx#0002</v>
       </c>
       <c r="F24" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E24)</f>
@@ -6121,7 +6120,7 @@
       </c>
       <c r="E25" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D25,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad6MCapletVolEx#0001</v>
+        <v>Cad6MCapletVolEx#0002</v>
       </c>
       <c r="F25" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E25)</f>
@@ -6140,7 +6139,7 @@
       </c>
       <c r="E26" s="18" t="str">
         <f>_xll.qlRelinkableHandleOptionletVolatilityStructure(D26,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Cad1YCapletVolEx#0001</v>
+        <v>Cad1YCapletVolEx#0002</v>
       </c>
       <c r="F26" s="20" t="str">
         <f>_xll.ohRangeRetrieveError(E26)</f>
@@ -6167,17 +6166,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>